<commit_message>
modified files ready for version 1.5
</commit_message>
<xml_diff>
--- a/klassegr/klassegrenser_PPBIOMTOVO.xlsx
+++ b/klassegr/klassegrenser_PPBIOMTOVO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nina\NatInd\2023\klassegr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NINA\OkoTilst\Pilot25\ecRxiv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F3FC3B-B82B-4376-AABE-2FE7F5E69433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E3817D-1E85-44E6-A5CD-C8EE4D76B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3A75F986-4B69-4A9F-BCAA-E28782105059}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3A75F986-4B69-4A9F-BCAA-E28782105059}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>typ</t>
   </si>
@@ -65,30 +65,6 @@
     <t>max</t>
   </si>
   <si>
-    <t>LN1</t>
-  </si>
-  <si>
-    <t>LN2a</t>
-  </si>
-  <si>
-    <t>LN2b</t>
-  </si>
-  <si>
-    <t>LN3</t>
-  </si>
-  <si>
-    <t>LN5</t>
-  </si>
-  <si>
-    <t>LN6</t>
-  </si>
-  <si>
-    <t>LN8</t>
-  </si>
-  <si>
-    <t>LN7</t>
-  </si>
-  <si>
     <t>L301</t>
   </si>
   <si>
@@ -105,6 +81,63 @@
   </si>
   <si>
     <t>L306</t>
+  </si>
+  <si>
+    <t>L107</t>
+  </si>
+  <si>
+    <t>L109</t>
+  </si>
+  <si>
+    <t>L104</t>
+  </si>
+  <si>
+    <t>L105a</t>
+  </si>
+  <si>
+    <t>L207</t>
+  </si>
+  <si>
+    <t>L105b</t>
+  </si>
+  <si>
+    <t>L106</t>
+  </si>
+  <si>
+    <t>L208</t>
+  </si>
+  <si>
+    <t>L101</t>
+  </si>
+  <si>
+    <t>L102</t>
+  </si>
+  <si>
+    <t>L201</t>
+  </si>
+  <si>
+    <t>L202</t>
+  </si>
+  <si>
+    <t>L204</t>
+  </si>
+  <si>
+    <t>L205</t>
+  </si>
+  <si>
+    <t>L103</t>
+  </si>
+  <si>
+    <t>L203</t>
+  </si>
+  <si>
+    <t>L206</t>
+  </si>
+  <si>
+    <t>L108</t>
+  </si>
+  <si>
+    <t>L110</t>
   </si>
 </sst>
 </file>
@@ -160,9 +193,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -200,7 +233,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -306,7 +339,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -448,7 +481,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -456,7 +489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA05597-937A-43B7-A68B-18184DD83021}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -493,7 +526,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>140</v>
@@ -522,28 +555,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>140</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>3.79</v>
+        <v>5.33</v>
       </c>
       <c r="E3">
-        <v>1.6</v>
+        <v>2.35</v>
       </c>
       <c r="F3">
+        <v>1.04</v>
+      </c>
+      <c r="G3">
         <v>0.64</v>
       </c>
-      <c r="G3">
-        <v>0.4</v>
-      </c>
       <c r="H3">
-        <v>0.18</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -551,28 +584,28 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>140</v>
       </c>
       <c r="C4">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>1.9</v>
+        <v>3.79</v>
       </c>
       <c r="E4">
-        <v>0.77</v>
+        <v>1.6</v>
       </c>
       <c r="F4">
-        <v>0.4</v>
+        <v>0.64</v>
       </c>
       <c r="G4">
-        <v>0.18</v>
+        <v>0.4</v>
       </c>
       <c r="H4">
-        <v>0.11</v>
+        <v>0.18</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -580,28 +613,28 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>140</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>4.5999999999999996</v>
+        <v>3.79</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.64</v>
       </c>
       <c r="G5">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="H5">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -609,28 +642,28 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>140</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>1.9</v>
+        <v>3.79</v>
       </c>
       <c r="E6">
-        <v>0.77</v>
+        <v>1.6</v>
       </c>
       <c r="F6">
-        <v>0.4</v>
+        <v>0.64</v>
       </c>
       <c r="G6">
-        <v>0.18</v>
+        <v>0.4</v>
       </c>
       <c r="H6">
-        <v>0.11</v>
+        <v>0.18</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -638,7 +671,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>140</v>
@@ -647,19 +680,19 @@
         <v>3.6</v>
       </c>
       <c r="D7">
-        <v>3.46</v>
+        <v>1.9</v>
       </c>
       <c r="E7">
-        <v>1.46</v>
+        <v>0.77</v>
       </c>
       <c r="F7">
-        <v>0.64</v>
+        <v>0.4</v>
       </c>
       <c r="G7">
-        <v>0.4</v>
+        <v>0.18</v>
       </c>
       <c r="H7">
-        <v>0.18</v>
+        <v>0.11</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -667,28 +700,28 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>140</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>6.03</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E8">
-        <v>2.66</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>1.24</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>0.77</v>
+        <v>0.6</v>
       </c>
       <c r="H8">
-        <v>0.34</v>
+        <v>0.3</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -696,28 +729,28 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>140</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>1.46</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E9">
-        <v>0.64</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>0.13</v>
+        <v>0.6</v>
       </c>
       <c r="H9">
-        <v>0.06</v>
+        <v>0.3</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -725,7 +758,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>140</v>
@@ -734,19 +767,19 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>1.46</v>
+        <v>1.9</v>
       </c>
       <c r="E10">
-        <v>0.64</v>
+        <v>0.77</v>
       </c>
       <c r="F10">
-        <v>0.23</v>
+        <v>0.4</v>
       </c>
       <c r="G10">
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="H10">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -754,7 +787,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>140</v>
@@ -763,19 +796,19 @@
         <v>3</v>
       </c>
       <c r="D11">
-        <v>1.46</v>
+        <v>1.9</v>
       </c>
       <c r="E11">
-        <v>0.64</v>
+        <v>0.77</v>
       </c>
       <c r="F11">
-        <v>0.23</v>
+        <v>0.4</v>
       </c>
       <c r="G11">
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="H11">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -783,7 +816,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>140</v>
@@ -792,19 +825,19 @@
         <v>3</v>
       </c>
       <c r="D12">
-        <v>1.46</v>
+        <v>1.9</v>
       </c>
       <c r="E12">
-        <v>0.64</v>
+        <v>0.77</v>
       </c>
       <c r="F12">
-        <v>0.23</v>
+        <v>0.4</v>
       </c>
       <c r="G12">
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="H12">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -812,7 +845,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>140</v>
@@ -821,19 +854,19 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>1.46</v>
+        <v>1.9</v>
       </c>
       <c r="E13">
-        <v>0.64</v>
+        <v>0.77</v>
       </c>
       <c r="F13">
-        <v>0.23</v>
+        <v>0.4</v>
       </c>
       <c r="G13">
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="H13">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -841,7 +874,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>140</v>
@@ -850,7 +883,7 @@
         <v>3</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="E14">
         <v>0.77</v>
@@ -870,7 +903,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>140</v>
@@ -879,7 +912,7 @@
         <v>3</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="E15">
         <v>0.77</v>
@@ -894,6 +927,325 @@
         <v>0.11</v>
       </c>
       <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16">
+        <v>140</v>
+      </c>
+      <c r="C16">
+        <v>3.6</v>
+      </c>
+      <c r="D16">
+        <v>3.46</v>
+      </c>
+      <c r="E16">
+        <v>1.46</v>
+      </c>
+      <c r="F16">
+        <v>0.64</v>
+      </c>
+      <c r="G16">
+        <v>0.4</v>
+      </c>
+      <c r="H16">
+        <v>0.18</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>140</v>
+      </c>
+      <c r="C17">
+        <v>3.6</v>
+      </c>
+      <c r="D17">
+        <v>3.46</v>
+      </c>
+      <c r="E17">
+        <v>1.46</v>
+      </c>
+      <c r="F17">
+        <v>0.64</v>
+      </c>
+      <c r="G17">
+        <v>0.4</v>
+      </c>
+      <c r="H17">
+        <v>0.18</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18">
+        <v>140</v>
+      </c>
+      <c r="C18">
+        <v>3.6</v>
+      </c>
+      <c r="D18">
+        <v>3.46</v>
+      </c>
+      <c r="E18">
+        <v>1.46</v>
+      </c>
+      <c r="F18">
+        <v>0.64</v>
+      </c>
+      <c r="G18">
+        <v>0.4</v>
+      </c>
+      <c r="H18">
+        <v>0.18</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>140</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>6.03</v>
+      </c>
+      <c r="E19">
+        <v>2.66</v>
+      </c>
+      <c r="F19">
+        <v>1.24</v>
+      </c>
+      <c r="G19">
+        <v>0.77</v>
+      </c>
+      <c r="H19">
+        <v>0.34</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>140</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>6.03</v>
+      </c>
+      <c r="E20">
+        <v>2.66</v>
+      </c>
+      <c r="F20">
+        <v>1.24</v>
+      </c>
+      <c r="G20">
+        <v>0.77</v>
+      </c>
+      <c r="H20">
+        <v>0.34</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>140</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>1.46</v>
+      </c>
+      <c r="E21">
+        <v>0.64</v>
+      </c>
+      <c r="F21">
+        <v>0.23</v>
+      </c>
+      <c r="G21">
+        <v>0.13</v>
+      </c>
+      <c r="H21">
+        <v>0.06</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>140</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>1.46</v>
+      </c>
+      <c r="E22">
+        <v>0.64</v>
+      </c>
+      <c r="F22">
+        <v>0.23</v>
+      </c>
+      <c r="G22">
+        <v>0.13</v>
+      </c>
+      <c r="H22">
+        <v>0.06</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>140</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>1.46</v>
+      </c>
+      <c r="E23">
+        <v>0.64</v>
+      </c>
+      <c r="F23">
+        <v>0.23</v>
+      </c>
+      <c r="G23">
+        <v>0.13</v>
+      </c>
+      <c r="H23">
+        <v>0.06</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>140</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>1.46</v>
+      </c>
+      <c r="E24">
+        <v>0.64</v>
+      </c>
+      <c r="F24">
+        <v>0.23</v>
+      </c>
+      <c r="G24">
+        <v>0.13</v>
+      </c>
+      <c r="H24">
+        <v>0.06</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>140</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0.77</v>
+      </c>
+      <c r="F25">
+        <v>0.4</v>
+      </c>
+      <c r="G25">
+        <v>0.18</v>
+      </c>
+      <c r="H25">
+        <v>0.11</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>140</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0.77</v>
+      </c>
+      <c r="F26">
+        <v>0.4</v>
+      </c>
+      <c r="G26">
+        <v>0.18</v>
+      </c>
+      <c r="H26">
+        <v>0.11</v>
+      </c>
+      <c r="I26">
         <v>0</v>
       </c>
     </row>

</xml_diff>